<commit_message>
Final OOPS version with Evaluation
</commit_message>
<xml_diff>
--- a/Codes/FIF_supervised Dataset.xlsx
+++ b/Codes/FIF_supervised Dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashis\Desktop\RToS\Codes\MicroService Architecture V 3.0\LDA_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashis\Desktop\RToS\Codes\MicroService Architecture V 3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0B7695-38F2-43E9-AED0-FBDCE167D884}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4541EA5A-5BA5-4C8D-A7B4-E14F100A9477}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="390" windowWidth="20445" windowHeight="10890" activeTab="1" xr2:uid="{4B496765-00C0-45E4-84B5-7DF728EC1A0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4B496765-00C0-45E4-84B5-7DF728EC1A0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Supervised" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Document 1</t>
   </si>
@@ -88,31 +88,25 @@
     <t>regression analyze regression category category category category separate segmentation</t>
   </si>
   <si>
-    <t>mean square correlation line error linear linear gradient</t>
-  </si>
-  <si>
-    <t>linear mean correlation line nonlinear SVR</t>
-  </si>
-  <si>
-    <t>mean root square correlation slope line error linear equation dimensionality soft epsilon</t>
-  </si>
-  <si>
-    <t>bias scatterplot SVM maximal margin nonlinear</t>
-  </si>
-  <si>
-    <t>gradient descent average scatterplot multipliers space feature vector</t>
-  </si>
-  <si>
-    <t>linear linear line linear support SVR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linear line line support vector SVR kernel kernel nonlinear </t>
-  </si>
-  <si>
-    <t>descent linear linear feature nonlinear nonlinear kernel dimensionality SVR SVM kernel nonlinear</t>
-  </si>
-  <si>
-    <t>nonlinear nonlinear nonlinear nonlinear kernel kernel SVM nonlinear kernel SVM</t>
+    <t xml:space="preserve">regression discrete linear observation analyse series </t>
+  </si>
+  <si>
+    <t>predict divided approximate range quantity labels class distribution statistics  analyse regression conitnous</t>
+  </si>
+  <si>
+    <t>classification category branch segmentation regression analyse  predict series</t>
+  </si>
+  <si>
+    <t>regression analyse regression predict series forecasting estimate count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regression analyse predict segmentation classification classification classification classification classification classification classification classification classification </t>
+  </si>
+  <si>
+    <t>regression regression analyse predict segmentation separate</t>
+  </si>
+  <si>
+    <t>regression analyse regression category category category category separate segmentation</t>
   </si>
 </sst>
 </file>
@@ -566,7 +560,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +606,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +614,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +630,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>